<commit_message>
update # of change points file
</commit_message>
<xml_diff>
--- a/modules/Trend Data & E.Divisive Algorithm/# change points.xlsx
+++ b/modules/Trend Data & E.Divisive Algorithm/# change points.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nielsmeulmeester/Documents/Education/Data Science/Courses/Master/Semester 2/Complex systems/Group Portfolio/e.divisive_entry/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3DF6AC78-B739-244B-9150-067292A7E0C9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6B3CA1B7-BDE5-4446-8235-CC02FD00E7B4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{CE5604FA-478F-804C-9B8B-77D2936FB6AE}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Sheep</t>
   </si>
@@ -46,9 +46,6 @@
   </si>
   <si>
     <t>trial 3</t>
-  </si>
-  <si>
-    <t>trial 4</t>
   </si>
 </sst>
 </file>
@@ -400,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6380D0AB-2A3D-BB43-BA1C-7BF685F31539}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -411,7 +408,7 @@
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -424,23 +421,47 @@
       <c r="D1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
+      <c r="B2">
+        <v>117</v>
+      </c>
+      <c r="C2">
+        <v>19</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
+      <c r="B3">
+        <v>108</v>
+      </c>
+      <c r="C3">
+        <v>16</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
+      </c>
+      <c r="B4">
+        <v>134</v>
+      </c>
+      <c r="C4">
+        <v>19</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>